<commit_message>
tweaked app for heroku
</commit_message>
<xml_diff>
--- a/Main Website/media/BAJAJ-CD/MIS/BAJAJ TC-WISE MIS.xlsx
+++ b/Main Website/media/BAJAJ-CD/MIS/BAJAJ TC-WISE MIS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,45 +461,50 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>EMPLOYEE_ID</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>MANAGER_ID</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>MANAGEMENT_LEVEL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>DESIGNATION</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>STAFF</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>EMPLOYEE_STATUS</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>PROCESS</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>DEPARTMENT</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>TYPE_OF_SALARY</t>
         </is>
@@ -523,43 +528,48 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
         <is>
           <t>O290</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
+          <t>O254</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>LOWER MANAGEMENT</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>OFFICE</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>ACTIVE</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>BAJAJ</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>CD</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>FIXED</t>
         </is>
@@ -583,43 +593,48 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
         <is>
           <t>O194</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
+          <t>O281</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>LOWER MANAGEMENT</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>OFFICE</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>ACTIVE</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>BAJAJ</t>
+          <t>INACTIVE</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>HERO</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
+        <is>
+          <t>RECOVERY</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>FIXED</t>
         </is>
@@ -643,47 +658,48 @@
       <c r="E4" t="n">
         <v>2500</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>O195</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>P200</t>
-        </is>
-      </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>O254</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>LOWER MANAGEMENT</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>OFFICE</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>ACTIVE</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>BAJAJ</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>CD</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>FIXED</t>
         </is>
@@ -707,47 +723,48 @@
       <c r="E5" t="n">
         <v>1500</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>O269</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>P200</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>O254</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>LOWER MANAGEMENT</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>OFFICE</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>ACTIVE</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>BAJAJ</t>
-        </is>
-      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>IDFC</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>FIXED</t>
         </is>

</xml_diff>